<commit_message>
Updating the PP with new tasks Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/Delivery History/Delivery History.xlsx
+++ b/Software Deliveries Log/Delivery History/Delivery History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\Delivery History\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF37074-2D06-4AE6-921E-ED771A963898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A22E5BC-D511-4B9D-A9DF-04B19140054B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{44ADEEAE-812D-4892-97CC-6D6F2881F008}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Digital Elevator_Delivery History</t>
   </si>
@@ -43,6 +43,33 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>Realasing the CYRS Document</t>
+  </si>
+  <si>
+    <t>Realasing the HSI Document</t>
+  </si>
+  <si>
+    <t>Realasing the SRS Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CYRS Document</t>
+  </si>
+  <si>
+    <t>HSI Document</t>
+  </si>
+  <si>
+    <t>SRS Document</t>
+  </si>
+  <si>
+    <t>CYRS_v1.5</t>
+  </si>
+  <si>
+    <t>SRS_v1.4</t>
+  </si>
+  <si>
+    <t>HSI_v1.3</t>
   </si>
 </sst>
 </file>
@@ -114,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,13 +158,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +545,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,18 +557,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -556,97 +586,120 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="C1:F2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D6:G6"/>
@@ -655,11 +708,9 @@
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="D11:G11"/>
-    <mergeCell ref="C1:F2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>